<commit_message>
impliment data driven testing using excel
</commit_message>
<xml_diff>
--- a/utils/testdata.xlsx
+++ b/utils/testdata.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rfnsh\PycharmProjects\mobileAutomationProject\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8546BB98-F0EC-4F65-9CF2-15C8EA3A4306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F45D575-3F71-4339-895A-BACC632258FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{466A1274-6B92-43C7-9BD7-72A0CCCEB455}"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="info" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>country</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>Male</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Dina</t>
+  </si>
+  <si>
+    <t>Female</t>
   </si>
 </sst>
 </file>
@@ -399,7 +408,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -432,6 +441,17 @@
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>